<commit_message>
Baseline model for patches and aggregation
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emman\OneDrive\Documents\Césure\Pays-Bas\PROT\PROT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deagogishvili/Documents/GitHub/chapter-multi-task/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D59E693-9827-40AA-B2C9-E901E75B9A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF11E57-82BD-B14C-A62A-EA0F3D18D864}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1500" windowWidth="22536" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="22540" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>SPARSE</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>SPARSE DECILE</t>
+  </si>
+  <si>
+    <t>AGG[95:96]</t>
+  </si>
+  <si>
+    <t>0 = NOT</t>
+  </si>
+  <si>
+    <t>1 = AGGREGATING</t>
   </si>
 </sst>
 </file>
@@ -453,37 +462,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="3" width="12.5546875" customWidth="1"/>
+    <col min="2" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
-    <col min="16" max="16" width="11.88671875" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
+    <col min="17" max="17" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="11.5" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.109375" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -547,8 +557,11 @@
       <c r="U1" t="s">
         <v>35</v>
       </c>
+      <c r="V1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -612,8 +625,11 @@
       <c r="U2" t="s">
         <v>36</v>
       </c>
+      <c r="V2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -628,6 +644,9 @@
       </c>
       <c r="R3" t="s">
         <v>29</v>
+      </c>
+      <c r="V3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>